<commit_message>
Created a test case excel document and fixed a bug for Search
- there was a bug where the number of events came up as 0 while searching. now loads events in Search
</commit_message>
<xml_diff>
--- a/TestCases cmpt370_group10.xlsx
+++ b/TestCases cmpt370_group10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13068\Desktop\Tyler_University\cmpt 370\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028B6377-1241-451F-9E15-06E0473A628B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907092E8-B5A9-427F-A9C6-1F3C68CF9D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7BED92FE-0701-4A75-A546-FB10C5E45C31}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="188">
   <si>
     <t>Test case ID</t>
   </si>
@@ -824,6 +824,127 @@
 for (int index = 0; index &lt; GetAllCueCards.size(); index++)
    System.out.println(GetNextCueCard())
 </t>
+  </si>
+  <si>
+    <t>Searching events and subjects for a 1</t>
+  </si>
+  <si>
+    <t>(1) added event with subject = a1
+(2) added event with subject = something</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events = [
+   {
+      subject = "a1"
+   },
+  {
+      subject = "something"
+   }
+]
+subjectList = [test subject 0, test subject 1, test subject 2]
+test subject 1:
+   currentCard = ["1 q3", 1 a3"]
+   cueCardList = [
+      {
+         question = "1 q1"
+         answer = "1 a1"
+      },
+      {
+         question = "1 q2"
+         answer = "1 a2"
+      },
+      {
+         question = "1 q3"
+         answer = "1 a3"
+      }
+   ]
+</t>
+  </si>
+  <si>
+    <t>To display information about the event with subject a 1 and the contents of the cue card in test subject 1 with an answer 1 a1</t>
+  </si>
+  <si>
+    <t>Events
+a1
+School
+900
+1000
+Subjects
+test subject 1
+cue cards that contain: a1:
+Question: 1 q1
+Answer: 1 a1</t>
+  </si>
+  <si>
+    <t>Saving and loading object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">devFolder = "Circle App/dev file"
+subjectList = [test subject 0, test subject 1, test subject 2]
+test subject 1:
+   currentCard = ["1 q3", 1 a3"]
+   cueCardList = [
+      {
+         question = "1 q1"
+         answer = "1 a1"
+      },
+      {
+         question = "1 q2"
+         answer = "1 a2"
+      },
+      {
+         question = "1 q3"
+         answer = "1 a3"
+      }
+   ]
+</t>
+  </si>
+  <si>
+    <t>SaveState.Save(devFolder + "/Subjects.json", subjectList)</t>
+  </si>
+  <si>
+    <t>Json file storing a list of subjects and their content</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "name": "test subject 0",
+    "filePath": "Circle App/test subject 0",
+    "notesPath": "Circle App/test subject 0/notes",
+    "cardPath": "Circle App/test subject 0/CueCards.json",
+    "cueCardsList": [],
+    "updated": true
+  },
+  {
+    "name": "test subject 1",
+    "filePath": "Circle App/test subject 1",
+    "notesPath": "Circle App/test subject 1/notes",
+    "cardPath": "Circle App/test subject 1/CueCards.json",
+    "cueCardsList": [
+      {
+        "question": "1 q1",
+        "answer": "1 a1"
+      },
+      {
+        "question": "1 q2",
+        "answer": "1 a2"
+      },
+      {
+        "question": "1 q3",
+        "answer": "1 a3"
+      }
+    ],
+    "updated": true
+  },
+  {
+    "name": "test subject 2",
+    "filePath": "Circle App/test subject 2",
+    "notesPath": "Circle App/test subject 2/notes",
+    "cardPath": "Circle App/test subject 2/CueCards.json",
+    "cueCardsList": [],
+    "updated": true
+  }
+]</t>
   </si>
 </sst>
 </file>
@@ -1224,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FA8D3F-76E8-423C-B5DB-D2344FF8783F}">
   <dimension ref="A1:G192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2048,23 +2169,47 @@
       <c r="A36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="300.14999999999998" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="300.14999999999998" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -3495,8 +3640,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>